<commit_message>
hrms payroll car omns
</commit_message>
<xml_diff>
--- a/ASP.NET CORE/HRMNS/Document HRMS/DichVietHan.xlsx
+++ b/ASP.NET CORE/HRMNS/Document HRMS/DichVietHan.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HIEU-UTI\UTI\EHS-Uti\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WorkSpace\Source\NET CORE\ASP.NET CORE\HRMNS\Document HRMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A0B1E1AA-968F-423A-99D7-405A07DEE812}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="144">
   <si>
     <t>Tên Tiếng Việt</t>
   </si>
@@ -358,12 +357,114 @@
   </si>
   <si>
     <t>권한 분할</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tiến độ </t>
+  </si>
+  <si>
+    <t>진도</t>
+  </si>
+  <si>
+    <t>Kết quả</t>
+  </si>
+  <si>
+    <t>결과</t>
+  </si>
+  <si>
+    <t>Đối sách cải tiến</t>
+  </si>
+  <si>
+    <t>개선대책</t>
+  </si>
+  <si>
+    <t>Theo dõi trên bảng công việc</t>
+  </si>
+  <si>
+    <t>업무표에 표시</t>
+  </si>
+  <si>
+    <t>Thông tin ngày bắt đầu,kết thúc và Import File Kết quả</t>
+  </si>
+  <si>
+    <t>시작일자, 종료일자 정보 및 결과 파일 import</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Danh Sách Nhân Viên Khám Sức Khỏe</t>
+  </si>
+  <si>
+    <t>건강검진 대상 명단</t>
+  </si>
+  <si>
+    <t>Hạng mục NG</t>
+  </si>
+  <si>
+    <t>NG항목</t>
+  </si>
+  <si>
+    <t>Nội dung NG</t>
+  </si>
+  <si>
+    <t>NG내용</t>
+  </si>
+  <si>
+    <t>Nguyên nhân NG</t>
+  </si>
+  <si>
+    <t>NG원인</t>
+  </si>
+  <si>
+    <t>Tình hình cải tiến</t>
+  </si>
+  <si>
+    <t>개선 현황</t>
+  </si>
+  <si>
+    <t>Quản lý các loại giấy phép</t>
+  </si>
+  <si>
+    <t>인허가 각종 관리</t>
+  </si>
+  <si>
+    <t>Lý do thực hiện</t>
+  </si>
+  <si>
+    <t>실시 사유</t>
+  </si>
+  <si>
+    <t>Theo dõi cơ quan nhà nước kiêm tra</t>
+  </si>
+  <si>
+    <t>국가기관 점검 이력 모니터링</t>
+  </si>
+  <si>
+    <t>Cơ quan kiểm tra</t>
+  </si>
+  <si>
+    <t>점검 기관명</t>
+  </si>
+  <si>
+    <t>Ngày kiểm tra</t>
+  </si>
+  <si>
+    <t>점검 일자</t>
+  </si>
+  <si>
+    <t>Nội dung kiểm tra</t>
+  </si>
+  <si>
+    <t>점검 내용</t>
+  </si>
+  <si>
+    <t>Hạng mục cải tiến NG</t>
+  </si>
+  <si>
+    <t>NG개선 항목</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -405,7 +506,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -413,9 +514,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -692,11 +796,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B59"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1146,8 +1250,144 @@
         <v>109</v>
       </c>
     </row>
+    <row r="61" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:B13" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:B13"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>